<commit_message>
files were refactored,gui initial
</commit_message>
<xml_diff>
--- a/src/resources/ІТтаКБ. Сем I. Форма навчання  заочна.xlsx
+++ b/src/resources/ІТтаКБ. Сем I. Форма навчання  заочна.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albru\PycharmProjects\StudyLoadPy1\src\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="516" yWindow="540" windowWidth="15996" windowHeight="7356"/>
   </bookViews>
@@ -10,15 +15,15 @@
     <sheet name="Робота кафедри" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Робота кафедри'!$A$1:$AG$56</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Робота кафедри'!$10:$17</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Робота кафедри'!$A$1:$AG$56</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="126">
   <si>
     <t>Затверджую</t>
   </si>
@@ -215,9 +220,6 @@
   </si>
   <si>
     <t xml:space="preserve">КН-740с2, КН-740с3, КН-740, </t>
-  </si>
-  <si>
-    <t>Крос-платформне програмування (КР)</t>
   </si>
   <si>
     <t>122(4к.)(1ч.)(3кр.)
@@ -421,7 +423,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -629,54 +631,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -691,17 +645,68 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -999,8 +1004,8 @@
   </sheetPr>
   <dimension ref="A1:AH56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG53" sqref="AG53"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="119" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1039,41 +1044,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="19"/>
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="20"/>
+      <c r="AG1" s="20"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
@@ -1081,27 +1086,27 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="28"/>
-      <c r="Z2" s="28"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
       <c r="AC2" s="4"/>
@@ -1111,615 +1116,615 @@
       <c r="AG2" s="4"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="28"/>
-      <c r="AA3" s="19"/>
-      <c r="AB3" s="19"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="19"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19"/>
-      <c r="AG3" s="19"/>
+      <c r="A3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="28"/>
-      <c r="W4" s="28"/>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="28"/>
-      <c r="Z4" s="28"/>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
-      <c r="AC4" s="19"/>
-      <c r="AD4" s="19"/>
-      <c r="AE4" s="19"/>
-      <c r="AF4" s="19"/>
-      <c r="AG4" s="19"/>
+      <c r="A4" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="18"/>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="20"/>
+      <c r="AC4" s="20"/>
+      <c r="AD4" s="20"/>
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="20"/>
+      <c r="AG4" s="20"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="25"/>
-      <c r="W5" s="25"/>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="25"/>
-      <c r="Z5" s="25"/>
-      <c r="AA5" s="25"/>
-      <c r="AB5" s="25"/>
-      <c r="AC5" s="26"/>
-      <c r="AD5" s="26"/>
-      <c r="AE5" s="26"/>
-      <c r="AF5" s="26"/>
-      <c r="AG5" s="26"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="24"/>
+      <c r="Z5" s="24"/>
+      <c r="AA5" s="24"/>
+      <c r="AB5" s="24"/>
+      <c r="AC5" s="23"/>
+      <c r="AD5" s="23"/>
+      <c r="AE5" s="23"/>
+      <c r="AF5" s="23"/>
+      <c r="AG5" s="23"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="25"/>
-      <c r="Y6" s="25"/>
-      <c r="Z6" s="25"/>
-      <c r="AA6" s="25"/>
-      <c r="AB6" s="25"/>
-      <c r="AC6" s="26"/>
-      <c r="AD6" s="26"/>
-      <c r="AE6" s="26"/>
-      <c r="AF6" s="26"/>
-      <c r="AG6" s="26"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="24"/>
+      <c r="AA6" s="24"/>
+      <c r="AB6" s="24"/>
+      <c r="AC6" s="23"/>
+      <c r="AD6" s="23"/>
+      <c r="AE6" s="23"/>
+      <c r="AF6" s="23"/>
+      <c r="AG6" s="23"/>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="19"/>
-      <c r="V7" s="19"/>
-      <c r="W7" s="19"/>
-      <c r="X7" s="19"/>
-      <c r="Y7" s="19"/>
-      <c r="Z7" s="19"/>
-      <c r="AA7" s="19"/>
-      <c r="AB7" s="20" t="s">
+      <c r="A7" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="20"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="AC7" s="20"/>
-      <c r="AD7" s="20"/>
-      <c r="AE7" s="20"/>
-      <c r="AF7" s="20"/>
-      <c r="AG7" s="20"/>
+      <c r="AC7" s="21"/>
+      <c r="AD7" s="21"/>
+      <c r="AE7" s="21"/>
+      <c r="AF7" s="21"/>
+      <c r="AG7" s="21"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="19"/>
-      <c r="V8" s="19"/>
-      <c r="W8" s="19"/>
-      <c r="X8" s="19"/>
-      <c r="Y8" s="19"/>
-      <c r="Z8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="20"/>
+      <c r="Z8" s="20"/>
       <c r="AA8" s="3"/>
-      <c r="AB8" s="20" t="s">
+      <c r="AB8" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="AC8" s="20"/>
-      <c r="AD8" s="20"/>
-      <c r="AE8" s="20"/>
-      <c r="AF8" s="20"/>
-      <c r="AG8" s="20"/>
+      <c r="AC8" s="21"/>
+      <c r="AD8" s="21"/>
+      <c r="AE8" s="21"/>
+      <c r="AF8" s="21"/>
+      <c r="AG8" s="21"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="26"/>
-      <c r="U9" s="26"/>
-      <c r="V9" s="26"/>
-      <c r="W9" s="26"/>
-      <c r="X9" s="26"/>
-      <c r="Y9" s="26"/>
-      <c r="Z9" s="26"/>
-      <c r="AA9" s="26"/>
-      <c r="AB9" s="26"/>
-      <c r="AC9" s="28"/>
-      <c r="AD9" s="28"/>
-      <c r="AE9" s="28"/>
-      <c r="AF9" s="28"/>
-      <c r="AG9" s="28"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="23"/>
+      <c r="Y9" s="23"/>
+      <c r="Z9" s="23"/>
+      <c r="AA9" s="23"/>
+      <c r="AB9" s="23"/>
+      <c r="AC9" s="18"/>
+      <c r="AD9" s="18"/>
+      <c r="AE9" s="18"/>
+      <c r="AF9" s="18"/>
+      <c r="AG9" s="18"/>
     </row>
     <row r="10" spans="1:33" s="1" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21" t="s">
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="21"/>
-      <c r="AC10" s="21"/>
-      <c r="AD10" s="21"/>
-      <c r="AE10" s="21"/>
-      <c r="AF10" s="21"/>
-      <c r="AG10" s="21"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22"/>
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="22"/>
+      <c r="AE10" s="22"/>
+      <c r="AF10" s="22"/>
+      <c r="AG10" s="22"/>
     </row>
     <row r="11" spans="1:33" s="1" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="21" t="s">
+      <c r="K11" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="21" t="s">
+      <c r="L11" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="M11" s="13" t="s">
+      <c r="M11" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="N11" s="21" t="s">
+      <c r="N11" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="O11" s="21" t="s">
+      <c r="O11" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="P11" s="21" t="s">
+      <c r="P11" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="21" t="s">
+      <c r="Q11" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="R11" s="21" t="s">
+      <c r="R11" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="S11" s="21" t="s">
+      <c r="S11" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="T11" s="21" t="s">
+      <c r="T11" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="U11" s="21" t="s">
+      <c r="U11" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="V11" s="21" t="s">
+      <c r="V11" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="W11" s="21" t="s">
+      <c r="W11" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="X11" s="16" t="s">
+      <c r="X11" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="Y11" s="17"/>
-      <c r="Z11" s="18"/>
-      <c r="AA11" s="21" t="s">
+      <c r="Y11" s="33"/>
+      <c r="Z11" s="34"/>
+      <c r="AA11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="AB11" s="21" t="s">
+      <c r="AB11" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="AC11" s="21" t="s">
+      <c r="AC11" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="AD11" s="21" t="s">
+      <c r="AD11" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="AE11" s="13" t="s">
+      <c r="AE11" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="AF11" s="22" t="s">
+      <c r="AF11" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="AG11" s="21" t="s">
+      <c r="AG11" s="22" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:33" s="1" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
-      <c r="T12" s="21"/>
-      <c r="U12" s="21"/>
-      <c r="V12" s="21"/>
-      <c r="W12" s="21"/>
-      <c r="X12" s="13" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="22"/>
+      <c r="U12" s="22"/>
+      <c r="V12" s="22"/>
+      <c r="W12" s="22"/>
+      <c r="X12" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="Y12" s="13" t="s">
+      <c r="Y12" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Z12" s="13" t="s">
+      <c r="Z12" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="AA12" s="21"/>
-      <c r="AB12" s="21"/>
-      <c r="AC12" s="21"/>
-      <c r="AD12" s="21"/>
-      <c r="AE12" s="14"/>
-      <c r="AF12" s="23"/>
-      <c r="AG12" s="21"/>
+      <c r="AA12" s="22"/>
+      <c r="AB12" s="22"/>
+      <c r="AC12" s="22"/>
+      <c r="AD12" s="22"/>
+      <c r="AE12" s="27"/>
+      <c r="AF12" s="30"/>
+      <c r="AG12" s="22"/>
     </row>
     <row r="13" spans="1:33" s="1" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="W13" s="21"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="21"/>
-      <c r="AB13" s="21"/>
-      <c r="AC13" s="21"/>
-      <c r="AD13" s="21"/>
-      <c r="AE13" s="14"/>
-      <c r="AF13" s="23"/>
-      <c r="AG13" s="21"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="22"/>
+      <c r="U13" s="22"/>
+      <c r="V13" s="22"/>
+      <c r="W13" s="22"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="27"/>
+      <c r="AA13" s="22"/>
+      <c r="AB13" s="22"/>
+      <c r="AC13" s="22"/>
+      <c r="AD13" s="22"/>
+      <c r="AE13" s="27"/>
+      <c r="AF13" s="30"/>
+      <c r="AG13" s="22"/>
     </row>
     <row r="14" spans="1:33" s="1" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="21"/>
-      <c r="W14" s="21"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="14"/>
-      <c r="AA14" s="21"/>
-      <c r="AB14" s="21"/>
-      <c r="AC14" s="21"/>
-      <c r="AD14" s="21"/>
-      <c r="AE14" s="14"/>
-      <c r="AF14" s="23"/>
-      <c r="AG14" s="21"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="22"/>
+      <c r="W14" s="22"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
+      <c r="Z14" s="27"/>
+      <c r="AA14" s="22"/>
+      <c r="AB14" s="22"/>
+      <c r="AC14" s="22"/>
+      <c r="AD14" s="22"/>
+      <c r="AE14" s="27"/>
+      <c r="AF14" s="30"/>
+      <c r="AG14" s="22"/>
     </row>
     <row r="15" spans="1:33" s="1" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="21"/>
-      <c r="W15" s="21"/>
-      <c r="X15" s="14"/>
-      <c r="Y15" s="14"/>
-      <c r="Z15" s="14"/>
-      <c r="AA15" s="21"/>
-      <c r="AB15" s="21"/>
-      <c r="AC15" s="21"/>
-      <c r="AD15" s="21"/>
-      <c r="AE15" s="14"/>
-      <c r="AF15" s="23"/>
-      <c r="AG15" s="21"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
+      <c r="T15" s="22"/>
+      <c r="U15" s="22"/>
+      <c r="V15" s="22"/>
+      <c r="W15" s="22"/>
+      <c r="X15" s="27"/>
+      <c r="Y15" s="27"/>
+      <c r="Z15" s="27"/>
+      <c r="AA15" s="22"/>
+      <c r="AB15" s="22"/>
+      <c r="AC15" s="22"/>
+      <c r="AD15" s="22"/>
+      <c r="AE15" s="27"/>
+      <c r="AF15" s="30"/>
+      <c r="AG15" s="22"/>
     </row>
     <row r="16" spans="1:33" s="1" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21"/>
-      <c r="U16" s="21"/>
-      <c r="V16" s="21"/>
-      <c r="W16" s="21"/>
-      <c r="X16" s="14"/>
-      <c r="Y16" s="14"/>
-      <c r="Z16" s="14"/>
-      <c r="AA16" s="21"/>
-      <c r="AB16" s="21"/>
-      <c r="AC16" s="21"/>
-      <c r="AD16" s="21"/>
-      <c r="AE16" s="14"/>
-      <c r="AF16" s="23"/>
-      <c r="AG16" s="21"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
+      <c r="U16" s="22"/>
+      <c r="V16" s="22"/>
+      <c r="W16" s="22"/>
+      <c r="X16" s="27"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="27"/>
+      <c r="AA16" s="22"/>
+      <c r="AB16" s="22"/>
+      <c r="AC16" s="22"/>
+      <c r="AD16" s="22"/>
+      <c r="AE16" s="27"/>
+      <c r="AF16" s="30"/>
+      <c r="AG16" s="22"/>
     </row>
     <row r="17" spans="1:33" s="1" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21"/>
-      <c r="U17" s="21"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="21"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
-      <c r="AA17" s="21"/>
-      <c r="AB17" s="21"/>
-      <c r="AC17" s="21"/>
-      <c r="AD17" s="21"/>
-      <c r="AE17" s="15"/>
-      <c r="AF17" s="24"/>
-      <c r="AG17" s="21"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="28"/>
+      <c r="Y17" s="28"/>
+      <c r="Z17" s="28"/>
+      <c r="AA17" s="22"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22"/>
+      <c r="AE17" s="28"/>
+      <c r="AF17" s="31"/>
+      <c r="AG17" s="22"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
@@ -1923,7 +1928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>3</v>
       </c>
@@ -2125,7 +2130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>5</v>
       </c>
@@ -2226,7 +2231,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <v>6</v>
       </c>
@@ -2327,7 +2332,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <v>7</v>
       </c>
@@ -2635,16 +2640,16 @@
         <v>10</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>64</v>
       </c>
       <c r="D27" s="10">
         <v>11</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F27" s="10">
         <v>1</v>
@@ -2668,7 +2673,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N27" s="10" t="s">
         <v>45</v>
@@ -2736,16 +2741,16 @@
         <v>11</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="D28" s="10">
+        <v>1</v>
+      </c>
+      <c r="E28" s="11" t="s">
         <v>68</v>
-      </c>
-      <c r="D28" s="10">
-        <v>1</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>69</v>
       </c>
       <c r="F28" s="10">
         <v>1</v>
@@ -2837,16 +2842,16 @@
         <v>12</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="D29" s="10">
+        <v>2</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>71</v>
-      </c>
-      <c r="D29" s="10">
-        <v>2</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>72</v>
       </c>
       <c r="F29" s="10">
         <v>1</v>
@@ -2938,16 +2943,16 @@
         <v>13</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="D30" s="10">
         <v>10</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F30" s="10">
         <v>1</v>
@@ -3039,7 +3044,7 @@
         <v>14</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>61</v>
@@ -3048,7 +3053,7 @@
         <v>11</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F31" s="10">
         <v>1</v>
@@ -3140,16 +3145,16 @@
         <v>15</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>79</v>
-      </c>
       <c r="D32" s="10">
         <v>1</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F32" s="10">
         <v>1</v>
@@ -3241,16 +3246,16 @@
         <v>16</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="D33" s="10">
         <v>10</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F33" s="10">
         <v>1</v>
@@ -3342,16 +3347,16 @@
         <v>17</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="10">
+        <v>1</v>
+      </c>
+      <c r="E34" s="11" t="s">
         <v>68</v>
-      </c>
-      <c r="D34" s="10">
-        <v>1</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>69</v>
       </c>
       <c r="F34" s="10">
         <v>1</v>
@@ -3443,16 +3448,16 @@
         <v>18</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>84</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>85</v>
       </c>
       <c r="D35" s="10">
         <v>7</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F35" s="10">
         <v>1</v>
@@ -3544,16 +3549,16 @@
         <v>19</v>
       </c>
       <c r="B36" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>88</v>
       </c>
       <c r="D36" s="10">
         <v>7</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F36" s="10">
         <v>1</v>
@@ -3645,16 +3650,16 @@
         <v>20</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D37" s="10">
         <v>7</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F37" s="10">
         <v>1</v>
@@ -3746,16 +3751,16 @@
         <v>21</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>90</v>
       </c>
       <c r="D38" s="10">
         <v>7</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F38" s="10">
         <v>1</v>
@@ -3847,16 +3852,16 @@
         <v>22</v>
       </c>
       <c r="B39" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="D39" s="10">
         <v>7</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F39" s="10">
         <v>1</v>
@@ -3948,16 +3953,16 @@
         <v>23</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="D40" s="10">
+        <v>4</v>
+      </c>
+      <c r="E40" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="D40" s="10">
-        <v>4</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>96</v>
       </c>
       <c r="F40" s="10">
         <v>1</v>
@@ -4049,16 +4054,16 @@
         <v>24</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="D41" s="10">
+        <v>4</v>
+      </c>
+      <c r="E41" s="11" t="s">
         <v>98</v>
-      </c>
-      <c r="D41" s="10">
-        <v>4</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>99</v>
       </c>
       <c r="F41" s="10">
         <v>1</v>
@@ -4150,16 +4155,16 @@
         <v>25</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="D42" s="10">
+        <v>1</v>
+      </c>
+      <c r="E42" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="D42" s="10">
-        <v>1</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>102</v>
       </c>
       <c r="F42" s="10">
         <v>1</v>
@@ -4186,7 +4191,7 @@
         <v>44</v>
       </c>
       <c r="N42" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O42" s="10" t="s">
         <v>45</v>
@@ -4251,16 +4256,16 @@
         <v>26</v>
       </c>
       <c r="B43" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C43" s="10" t="s">
-        <v>105</v>
-      </c>
       <c r="D43" s="10">
         <v>4</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F43" s="10">
         <v>1</v>
@@ -4352,16 +4357,16 @@
         <v>27</v>
       </c>
       <c r="B44" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="D44" s="10">
+        <v>2</v>
+      </c>
+      <c r="E44" s="11" t="s">
         <v>107</v>
-      </c>
-      <c r="D44" s="10">
-        <v>2</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>108</v>
       </c>
       <c r="F44" s="10">
         <v>1</v>
@@ -4453,16 +4458,16 @@
         <v>28</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>110</v>
-      </c>
       <c r="D45" s="10">
         <v>2</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F45" s="10">
         <v>1</v>
@@ -4554,16 +4559,16 @@
         <v>29</v>
       </c>
       <c r="B46" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="10" t="s">
-        <v>112</v>
-      </c>
       <c r="D46" s="10">
         <v>4</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F46" s="10">
         <v>1</v>
@@ -4655,16 +4660,16 @@
         <v>30</v>
       </c>
       <c r="B47" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C47" s="10" t="s">
-        <v>114</v>
-      </c>
       <c r="D47" s="10">
         <v>2</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F47" s="10">
         <v>1</v>
@@ -4756,16 +4761,16 @@
         <v>31</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="D48" s="10">
+        <v>1</v>
+      </c>
+      <c r="E48" s="11" t="s">
         <v>116</v>
-      </c>
-      <c r="D48" s="10">
-        <v>1</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>117</v>
       </c>
       <c r="F48" s="10">
         <v>1</v>
@@ -4857,16 +4862,16 @@
         <v>32</v>
       </c>
       <c r="B49" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" s="10" t="s">
         <v>118</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>119</v>
       </c>
       <c r="D49" s="10">
         <v>3</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F49" s="10">
         <v>1</v>
@@ -4958,16 +4963,16 @@
         <v>33</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D50" s="10">
         <v>3</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F50" s="10">
         <v>1</v>
@@ -5094,7 +5099,7 @@
         <v>34</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
@@ -5131,13 +5136,13 @@
       </c>
     </row>
     <row r="53" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A53" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="B53" s="30"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="31"/>
+      <c r="A53" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B53" s="14"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
       <c r="F53" s="12">
         <v>33</v>
       </c>
@@ -5212,14 +5217,14 @@
       </c>
     </row>
     <row r="54" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A54" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="B54" s="30"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="32"/>
+      <c r="A54" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B54" s="14"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="16"/>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
@@ -5277,46 +5282,85 @@
       </c>
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A56" s="33" t="s">
+      <c r="A56" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B56" s="18"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="17"/>
+      <c r="P56" s="17"/>
+      <c r="Q56" s="17"/>
+      <c r="S56" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="B56" s="28"/>
-      <c r="C56" s="33"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="33"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="33"/>
-      <c r="H56" s="33"/>
-      <c r="I56" s="33"/>
-      <c r="J56" s="33"/>
-      <c r="K56" s="33"/>
-      <c r="L56" s="33"/>
-      <c r="M56" s="33"/>
-      <c r="N56" s="33"/>
-      <c r="O56" s="33"/>
-      <c r="P56" s="33"/>
-      <c r="Q56" s="33"/>
-      <c r="S56" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="T56" s="33"/>
-      <c r="U56" s="33"/>
-      <c r="V56" s="33"/>
-      <c r="W56" s="33"/>
-      <c r="X56" s="33"/>
-      <c r="Y56" s="33"/>
-      <c r="Z56" s="33"/>
-      <c r="AA56" s="33"/>
-      <c r="AB56" s="33"/>
-      <c r="AC56" s="33"/>
-      <c r="AD56" s="33"/>
-      <c r="AE56" s="33"/>
-      <c r="AF56" s="33"/>
-      <c r="AG56" s="33"/>
+      <c r="T56" s="17"/>
+      <c r="U56" s="17"/>
+      <c r="V56" s="17"/>
+      <c r="W56" s="17"/>
+      <c r="X56" s="17"/>
+      <c r="Y56" s="17"/>
+      <c r="Z56" s="17"/>
+      <c r="AA56" s="17"/>
+      <c r="AB56" s="17"/>
+      <c r="AC56" s="17"/>
+      <c r="AD56" s="17"/>
+      <c r="AE56" s="17"/>
+      <c r="AF56" s="17"/>
+      <c r="AG56" s="17"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="55">
+    <mergeCell ref="N11:N17"/>
+    <mergeCell ref="O11:O17"/>
+    <mergeCell ref="M11:M17"/>
+    <mergeCell ref="X11:Z11"/>
+    <mergeCell ref="X12:X17"/>
+    <mergeCell ref="Y12:Y17"/>
+    <mergeCell ref="Z12:Z17"/>
+    <mergeCell ref="AE11:AE17"/>
+    <mergeCell ref="AF11:AF17"/>
+    <mergeCell ref="A7:AA7"/>
+    <mergeCell ref="AB7:AG7"/>
+    <mergeCell ref="H10:H17"/>
+    <mergeCell ref="I11:I17"/>
+    <mergeCell ref="J11:J17"/>
+    <mergeCell ref="K11:K17"/>
+    <mergeCell ref="L11:L17"/>
+    <mergeCell ref="P11:P17"/>
+    <mergeCell ref="Q11:Q17"/>
+    <mergeCell ref="R11:R17"/>
+    <mergeCell ref="S11:S17"/>
+    <mergeCell ref="T11:T17"/>
+    <mergeCell ref="V11:V17"/>
+    <mergeCell ref="U11:U17"/>
+    <mergeCell ref="AD11:AD17"/>
+    <mergeCell ref="G10:G17"/>
+    <mergeCell ref="I10:O10"/>
+    <mergeCell ref="P10:AG10"/>
+    <mergeCell ref="AA1:AG1"/>
+    <mergeCell ref="AA3:AG3"/>
+    <mergeCell ref="AA4:AG4"/>
+    <mergeCell ref="A5:AB6"/>
+    <mergeCell ref="AC5:AG6"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F1:Z4"/>
+    <mergeCell ref="AG11:AG17"/>
+    <mergeCell ref="W11:W17"/>
+    <mergeCell ref="AA11:AA17"/>
     <mergeCell ref="A53:E53"/>
     <mergeCell ref="A54:F54"/>
     <mergeCell ref="A56:Q56"/>
@@ -5333,47 +5377,8 @@
     <mergeCell ref="A10:A17"/>
     <mergeCell ref="AB11:AB17"/>
     <mergeCell ref="AC11:AC17"/>
-    <mergeCell ref="AD11:AD17"/>
-    <mergeCell ref="G10:G17"/>
-    <mergeCell ref="I10:O10"/>
-    <mergeCell ref="P10:AG10"/>
-    <mergeCell ref="AA1:AG1"/>
-    <mergeCell ref="AA3:AG3"/>
-    <mergeCell ref="AA4:AG4"/>
-    <mergeCell ref="A5:AB6"/>
-    <mergeCell ref="AC5:AG6"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F1:Z4"/>
-    <mergeCell ref="AG11:AG17"/>
-    <mergeCell ref="W11:W17"/>
-    <mergeCell ref="AA11:AA17"/>
-    <mergeCell ref="AE11:AE17"/>
-    <mergeCell ref="AF11:AF17"/>
-    <mergeCell ref="A7:AA7"/>
-    <mergeCell ref="AB7:AG7"/>
-    <mergeCell ref="H10:H17"/>
-    <mergeCell ref="I11:I17"/>
-    <mergeCell ref="J11:J17"/>
-    <mergeCell ref="K11:K17"/>
-    <mergeCell ref="L11:L17"/>
-    <mergeCell ref="P11:P17"/>
-    <mergeCell ref="Q11:Q17"/>
-    <mergeCell ref="R11:R17"/>
-    <mergeCell ref="S11:S17"/>
-    <mergeCell ref="T11:T17"/>
-    <mergeCell ref="V11:V17"/>
-    <mergeCell ref="U11:U17"/>
-    <mergeCell ref="N11:N17"/>
-    <mergeCell ref="O11:O17"/>
-    <mergeCell ref="M11:M17"/>
-    <mergeCell ref="X11:Z11"/>
-    <mergeCell ref="X12:X17"/>
-    <mergeCell ref="Y12:Y17"/>
-    <mergeCell ref="Z12:Z17"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="1.37795" bottom="0" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>